<commit_message>
Feat keywords and descriptions creation
</commit_message>
<xml_diff>
--- a/excel-files/examples/keywords-template.xlsx
+++ b/excel-files/examples/keywords-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geffe\Desktop\codigo\vtex-wizard\excel-files\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15975822-5419-4912-97CA-0CE8579E308F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D53C60E-07EA-4AAB-AE5C-EF5088804419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BB6D2A9F-B0F7-4840-8DFF-3CA20C555DC5}"/>
   </bookViews>
@@ -36,37 +36,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Cubiertos Parrilleros Behome</t>
-  </si>
-  <si>
-    <t>Menaje Cocina</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Categoria</t>
   </si>
   <si>
     <t>Nombre</t>
+  </si>
+  <si>
+    <t>Marca</t>
+  </si>
+  <si>
+    <t>Mesa de Centro Moderna Montego 1 Cajón</t>
+  </si>
+  <si>
+    <t>TU MESITA</t>
+  </si>
+  <si>
+    <t>Sala</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,10 +89,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,35 +426,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9981B8-0A8C-4140-8339-1132395B1CCC}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="42.77734375" customWidth="1"/>
+    <col min="1" max="2" width="42.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>